<commit_message>
Avances al 4 de marzo
Añade los informes de análisis cuali aun x corregir
</commit_message>
<xml_diff>
--- a/clasificación de reclamos.xlsx
+++ b/clasificación de reclamos.xlsx
@@ -27,23 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
-  <si>
-    <t>Categorias</t>
-  </si>
-  <si>
-    <t>Items</t>
-  </si>
-  <si>
-    <t>Problemas de Infraestructura y/o moviliario</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Deficiencias en el orden y limpieza de la infraestructura de la IPRESS</t>
   </si>
   <si>
-    <t>Deficiencia o falta de infraestructura y/o moviliario</t>
-  </si>
-  <si>
     <t>Problemas del Seguro (SIS)</t>
   </si>
   <si>
@@ -77,12 +65,6 @@
     <t>Información errada, insuficiente, no comprensible u omitida sobre procedimientos, diagnosticos y/o tratamiento medico</t>
   </si>
   <si>
-    <t>Información errada, insuficiente, no comprensible u omitida sobre la atención en salud</t>
-  </si>
-  <si>
-    <t>Cobros no autorizados en el procedimiento realizado</t>
-  </si>
-  <si>
     <t>Información errada, insuficiente, no comprensible u omitida sobre el personal asistencial</t>
   </si>
   <si>
@@ -146,9 +128,6 @@
     <t>Incumplimiento de citas</t>
   </si>
   <si>
-    <t>Demora de citas</t>
-  </si>
-  <si>
     <t>Falta de citas</t>
   </si>
   <si>
@@ -158,9 +137,6 @@
     <t>Disconformidad de la atención y/o tratamiento medico ambulatorio, domiciliario y/o emergencia</t>
   </si>
   <si>
-    <t>Disconformidad con la atención a domicilio</t>
-  </si>
-  <si>
     <t>Disconformidad relacionada a la atención en hospitalización</t>
   </si>
   <si>
@@ -176,9 +152,6 @@
     <t>Disconformidad con la referencia y/o traslado</t>
   </si>
   <si>
-    <t>Demora en la referencia u procedimientp</t>
-  </si>
-  <si>
     <t>Incumplimiento del horario de atención</t>
   </si>
   <si>
@@ -194,9 +167,6 @@
     <t>Demora en la entrega de documentos (recetas, ordenes, altas, certificados, etc.)</t>
   </si>
   <si>
-    <t>Demora en entrega de carta garantia</t>
-  </si>
-  <si>
     <t>Demora en la atención al usuario por telefono</t>
   </si>
   <si>
@@ -218,17 +188,30 @@
     <t>Demora en el proceso de admisión del asegurado (por personal no medico)</t>
   </si>
   <si>
-    <t>No va</t>
+    <t>Problemas de Infraestructura y/o mobiliario</t>
+  </si>
+  <si>
+    <t>Deficiencia o falta de infraestructura y/o mobiliario</t>
+  </si>
+  <si>
+    <t>Categorias / Items</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -261,11 +244,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -273,7 +260,56 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -281,6 +317,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A3:K12" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A3:K12"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Categorias / Items"/>
+    <tableColumn id="2" name="Problemas de Infraestructura y/o mobiliario" dataDxfId="10"/>
+    <tableColumn id="3" name="Problemas del Seguro (SIS)" dataDxfId="9"/>
+    <tableColumn id="4" name="Privacidad y Confidencialidad del Asegurado" dataDxfId="8"/>
+    <tableColumn id="5" name="Problemas en Información"/>
+    <tableColumn id="6" name="Historia Clinica" dataDxfId="7"/>
+    <tableColumn id="7" name="Problemas con Medicamentos, Insumos y/o reactivos" dataDxfId="6"/>
+    <tableColumn id="8" name="Problemas con el trato al asegurado" dataDxfId="5"/>
+    <tableColumn id="9" name="Problemas con las citas" dataDxfId="4"/>
+    <tableColumn id="10" name="Problemas en la atención al paciente" dataDxfId="3"/>
+    <tableColumn id="11" name="Demoras" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -546,242 +602,252 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L13"/>
+  <dimension ref="A3:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:K13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="39.5" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="47.1640625" customWidth="1"/>
+    <col min="8" max="8" width="32.83203125" customWidth="1"/>
+    <col min="9" max="9" width="22.5" customWidth="1"/>
+    <col min="10" max="10" width="33.5" customWidth="1"/>
     <col min="11" max="11" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="112" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="I5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="80" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -790,14 +856,17 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1" t="s">
-        <v>49</v>
+      <c r="J11" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -806,14 +875,11 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="144" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -822,14 +888,11 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>62</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios al 30 de Marzo
Se actualizaron las correcciones de ccc en recomendaciones y
conclusiones. Se hicieron algunas modificaciones en discusión y
resultados, falta terminar esto. Falta resumen.
</commit_message>
<xml_diff>
--- a/clasificación de reclamos.xlsx
+++ b/clasificación de reclamos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="24560" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="180" yWindow="440" windowWidth="24560" windowHeight="14320" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="88">
   <si>
     <t>Deficiencias en el orden y limpieza de la infraestructura de la IPRESS</t>
   </si>
@@ -195,13 +197,109 @@
   </si>
   <si>
     <t>Categorias / Items</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Item #1</t>
+  </si>
+  <si>
+    <t>Item #2</t>
+  </si>
+  <si>
+    <t>Mal manejo de Historia Clinica (maltrato, mal compaginamiento, legibilidad, etc.)</t>
+  </si>
+  <si>
+    <t>Item #3</t>
+  </si>
+  <si>
+    <t>Item #4</t>
+  </si>
+  <si>
+    <t>Item #5</t>
+  </si>
+  <si>
+    <t>Item #6</t>
+  </si>
+  <si>
+    <t>Item #7</t>
+  </si>
+  <si>
+    <t>Item #8</t>
+  </si>
+  <si>
+    <t>Item #9</t>
+  </si>
+  <si>
+    <t>Categoría</t>
+  </si>
+  <si>
+    <t>Presencia de personal no autorizado por el usuario en la evaluación médica</t>
+  </si>
+  <si>
+    <t>Falta y/o violación de la confidencialidad del asegurado (Refiriéndose a datos, diagnóstico y/o material multimedia)</t>
+  </si>
+  <si>
+    <t>Información errada, insuficiente, no comprensible u omitida sobre procedimientos, diagnósticos y/o tratamiento médico</t>
+  </si>
+  <si>
+    <t>Información errada, insuficiente, no comprensible u omitida sobre procedimientos asistenciales no médicos (exámenes de laboratorio, etc.)</t>
+  </si>
+  <si>
+    <t>Historia Clínica</t>
+  </si>
+  <si>
+    <t>Perdida de Historia Clínica</t>
+  </si>
+  <si>
+    <t>Duplicidad de Historia Clínica</t>
+  </si>
+  <si>
+    <t>Mal manejo de Historia Clínica (maltrato, mal compaginamiento, ilegibilidad, etc.)</t>
+  </si>
+  <si>
+    <t>Descortesía del personal no médico</t>
+  </si>
+  <si>
+    <t>Descortesía del personal médico</t>
+  </si>
+  <si>
+    <t>Descortesía del personal administrativo</t>
+  </si>
+  <si>
+    <t>Disconformidad de la atención y/o tratamiento médico ambulatorio, domiciliario y/o emergencia</t>
+  </si>
+  <si>
+    <t>Mal diagnóstico o procedimiento que ponga en riesgo la vida del paciente (por parte del Personal Asistencial)</t>
+  </si>
+  <si>
+    <t>Cambio de médico tratante de forma arbitraria</t>
+  </si>
+  <si>
+    <t>Disconformidad con los procedimientos administrativos realizados</t>
+  </si>
+  <si>
+    <t>Demora en la entrega de documentos (recetas, órdenes, altas, certificados, etc.)</t>
+  </si>
+  <si>
+    <t>Demora en la atención al usuario por teléfono</t>
+  </si>
+  <si>
+    <t>Demora en la realización de exámenes</t>
+  </si>
+  <si>
+    <t>Demora en la intervención quirúrgica</t>
+  </si>
+  <si>
+    <t>Demora en el proceso de admisión del asegurado (por personal no médico)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,16 +321,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -240,11 +382,118 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -256,27 +505,66 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -307,6 +595,21 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -315,25 +618,28 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A3:K12" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A3:K12" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A3:K12"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Categorias / Items"/>
-    <tableColumn id="2" name="Problemas de Infraestructura y/o mobiliario" dataDxfId="10"/>
-    <tableColumn id="3" name="Problemas del Seguro (SIS)" dataDxfId="9"/>
-    <tableColumn id="4" name="Privacidad y Confidencialidad del Asegurado" dataDxfId="8"/>
+    <tableColumn id="2" name="Problemas de Infraestructura y/o mobiliario" dataDxfId="8"/>
+    <tableColumn id="3" name="Problemas del Seguro (SIS)" dataDxfId="7"/>
+    <tableColumn id="4" name="Privacidad y Confidencialidad del Asegurado" dataDxfId="6"/>
     <tableColumn id="5" name="Problemas en Información"/>
-    <tableColumn id="6" name="Historia Clinica" dataDxfId="7"/>
-    <tableColumn id="7" name="Problemas con Medicamentos, Insumos y/o reactivos" dataDxfId="6"/>
-    <tableColumn id="8" name="Problemas con el trato al asegurado" dataDxfId="5"/>
-    <tableColumn id="9" name="Problemas con las citas" dataDxfId="4"/>
-    <tableColumn id="10" name="Problemas en la atención al paciente" dataDxfId="3"/>
-    <tableColumn id="11" name="Demoras" dataDxfId="2"/>
+    <tableColumn id="6" name="Historia Clinica" dataDxfId="5"/>
+    <tableColumn id="7" name="Problemas con Medicamentos, Insumos y/o reactivos" dataDxfId="4"/>
+    <tableColumn id="8" name="Problemas con el trato al asegurado" dataDxfId="3"/>
+    <tableColumn id="9" name="Problemas con las citas" dataDxfId="2"/>
+    <tableColumn id="10" name="Problemas en la atención al paciente" dataDxfId="1"/>
+    <tableColumn id="11" name="Demoras" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -604,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,7 +964,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -728,7 +1034,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -758,7 +1064,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -783,7 +1089,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -844,7 +1150,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -895,4 +1201,928 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="59.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="78" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B15" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B18" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="28"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B39" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B40" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B41" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B42" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B45" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B47" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B48" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B49" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B50" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B51" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B52" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B53" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B54" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B55" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+</worksheet>
 </file>
</xml_diff>